<commit_message>
Change the output policy
Output YAML file will be output as one file including all sheet.
</commit_message>
<xml_diff>
--- a/sample_data/sample_device.xlsx
+++ b/sample_data/sample_device.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>10.1.1.1</t>
     <phoneticPr fontId="1"/>
@@ -185,8 +185,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -213,7 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -222,6 +224,7 @@
     <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -231,6 +234,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -561,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -843,98 +847,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
+    <row r="1" spans="1:7" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="3" customFormat="1">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>